<commit_message>
renta imputada para casa cedida o prestada
</commit_message>
<xml_diff>
--- a/poverty_measurement/output/canasta_diaria.xlsx
+++ b/poverty_measurement/output/canasta_diaria.xlsx
@@ -33,12 +33,12 @@
     <t>Queso blanco</t>
   </si>
   <si>
+    <t>Pastas alimenticias</t>
+  </si>
+  <si>
     <t>Yuca</t>
   </si>
   <si>
-    <t>Pastas alimenticias</t>
-  </si>
-  <si>
     <t>Carne de res (bistec, carne molida, carne para esmechar)</t>
   </si>
   <si>
@@ -57,19 +57,19 @@
     <t>Carne de pollo</t>
   </si>
   <si>
+    <t>Frijoles</t>
+  </si>
+  <si>
     <t>Platanos</t>
   </si>
   <si>
-    <t>Frijoles</t>
-  </si>
-  <si>
     <t>Huevos (unidades)</t>
   </si>
   <si>
+    <t>Caraotas</t>
+  </si>
+  <si>
     <t>Leche en polvo, completa o descremada</t>
-  </si>
-  <si>
-    <t>Caraotas</t>
   </si>
   <si>
     <t>Pescado fresco</t>
@@ -188,19 +188,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>95.787974577537199</v>
+        <v>94.976976093559728</v>
       </c>
       <c r="C2" s="1">
-        <v>118.14552434073907</v>
+        <v>117.96357444086199</v>
       </c>
       <c r="D2" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E2" s="1">
         <v>383</v>
       </c>
       <c r="F2" s="1">
-        <v>452.49734497070313</v>
+        <v>451.80047607421875</v>
       </c>
     </row>
     <row r="3">
@@ -208,19 +208,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>87.884480274219484</v>
+        <v>88.071501905872964</v>
       </c>
       <c r="C3" s="1">
-        <v>108.39730193634794</v>
+        <v>109.386817814227</v>
       </c>
       <c r="D3" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E3" s="1">
         <v>345</v>
       </c>
       <c r="F3" s="1">
-        <v>373.970703125</v>
+        <v>377.384521484375</v>
       </c>
     </row>
     <row r="4">
@@ -228,19 +228,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>20.403670383610464</v>
+        <v>19.665394595351557</v>
       </c>
       <c r="C4" s="1">
-        <v>25.166022296534997</v>
+        <v>24.424869165146379</v>
       </c>
       <c r="D4" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E4" s="1">
         <v>900</v>
       </c>
       <c r="F4" s="1">
-        <v>226.49420166015625</v>
+        <v>219.82382202148438</v>
       </c>
     </row>
     <row r="5">
@@ -248,19 +248,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>29.412884149059479</v>
+        <v>29.394199233785663</v>
       </c>
       <c r="C5" s="1">
-        <v>36.278047371862733</v>
+        <v>36.50826673041788</v>
       </c>
       <c r="D5" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E5" s="1">
         <v>393.5</v>
       </c>
       <c r="F5" s="1">
-        <v>142.75411987304688</v>
+        <v>143.6600341796875</v>
       </c>
     </row>
     <row r="6">
@@ -268,19 +268,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>20.212503545891227</v>
+        <v>20.209372464348288</v>
       </c>
       <c r="C6" s="1">
-        <v>24.930236534588349</v>
+        <v>25.100502154881791</v>
       </c>
       <c r="D6" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E6" s="1">
         <v>368.5</v>
       </c>
       <c r="F6" s="1">
-        <v>91.867919921875</v>
+        <v>92.495353698730469</v>
       </c>
     </row>
     <row r="7">
@@ -288,19 +288,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>36.800571349297904</v>
+        <v>45.010208802747741</v>
       </c>
       <c r="C7" s="1">
-        <v>45.390069489947173</v>
+        <v>55.903707537868165</v>
       </c>
       <c r="D7" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E7" s="1">
-        <v>182.33332824707031</v>
+        <v>137.5</v>
       </c>
       <c r="F7" s="1">
-        <v>82.761222839355469</v>
+        <v>76.867599487304688</v>
       </c>
     </row>
     <row r="8">
@@ -308,19 +308,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>42.724032615306172</v>
+        <v>33.815221819460845</v>
       </c>
       <c r="C8" s="1">
-        <v>52.696106145544576</v>
+        <v>41.999278094214674</v>
       </c>
       <c r="D8" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E8" s="1">
-        <v>137.5</v>
+        <v>182.33332824707031</v>
       </c>
       <c r="F8" s="1">
-        <v>72.457145690917969</v>
+        <v>76.578681945800781</v>
       </c>
     </row>
     <row r="9">
@@ -328,19 +328,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>28.83527537042805</v>
+        <v>28.417130347936801</v>
       </c>
       <c r="C9" s="1">
-        <v>35.565620607068254</v>
+        <v>35.294724975007838</v>
       </c>
       <c r="D9" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E9" s="1">
         <v>196.5</v>
       </c>
       <c r="F9" s="1">
-        <v>69.886444091796875</v>
+        <v>69.354133605957031</v>
       </c>
     </row>
     <row r="10">
@@ -348,19 +348,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>13.610649013360606</v>
+        <v>14.018136161076503</v>
       </c>
       <c r="C10" s="1">
-        <v>16.787465095202656</v>
+        <v>17.410845444581959</v>
       </c>
       <c r="D10" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E10" s="1">
         <v>355</v>
       </c>
       <c r="F10" s="1">
-        <v>59.595500946044922</v>
+        <v>61.808502197265625</v>
       </c>
     </row>
     <row r="11">
@@ -368,19 +368,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>17.043024029152566</v>
+        <v>17.566349087224207</v>
       </c>
       <c r="C11" s="1">
-        <v>21.020979448721533</v>
+        <v>21.817806737056085</v>
       </c>
       <c r="D11" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E11" s="1">
         <v>254.5</v>
       </c>
       <c r="F11" s="1">
-        <v>53.498394012451172</v>
+        <v>55.526317596435547</v>
       </c>
     </row>
     <row r="12">
@@ -388,19 +388,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>5.8754458267954544</v>
+        <v>5.620282138927152</v>
       </c>
       <c r="C12" s="1">
-        <v>7.2468140628294222</v>
+        <v>6.9805187861283144</v>
       </c>
       <c r="D12" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E12" s="1">
         <v>584</v>
       </c>
       <c r="F12" s="1">
-        <v>42.321395874023438</v>
+        <v>40.766231536865234</v>
       </c>
     </row>
     <row r="13">
@@ -408,19 +408,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>29.441930917495498</v>
+        <v>28.7704038673875</v>
       </c>
       <c r="C13" s="1">
-        <v>36.313873505552678</v>
+        <v>35.733498839216402</v>
       </c>
       <c r="D13" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E13" s="1">
         <v>113.375</v>
       </c>
       <c r="F13" s="1">
-        <v>41.170852661132813</v>
+        <v>40.512855529785156</v>
       </c>
     </row>
     <row r="14">
@@ -428,19 +428,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>17.594010477970524</v>
+        <v>18.268528258614303</v>
       </c>
       <c r="C14" s="1">
-        <v>21.700569698695535</v>
+        <v>22.689929412583172</v>
       </c>
       <c r="D14" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E14" s="1">
         <v>174</v>
       </c>
       <c r="F14" s="1">
-        <v>37.758991241455078</v>
+        <v>39.480476379394531</v>
       </c>
     </row>
     <row r="15">
@@ -448,19 +448,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>17.120513725280762</v>
+        <v>7.4372123992098409</v>
       </c>
       <c r="C15" s="1">
-        <v>21.116555751857664</v>
+        <v>9.2371876337235843</v>
       </c>
       <c r="D15" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E15" s="1">
-        <v>164.85714721679688</v>
+        <v>405.84616088867188</v>
       </c>
       <c r="F15" s="1">
-        <v>34.812152862548828</v>
+        <v>37.48876953125</v>
       </c>
     </row>
     <row r="16">
@@ -468,19 +468,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>6.8718804088091092</v>
+        <v>16.781085621918425</v>
       </c>
       <c r="C16" s="1">
-        <v>8.475823121538971</v>
+        <v>20.842491949860459</v>
       </c>
       <c r="D16" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E16" s="1">
-        <v>405.84616088867188</v>
+        <v>164.85714721679688</v>
       </c>
       <c r="F16" s="1">
-        <v>34.3988037109375</v>
+        <v>34.360336303710938</v>
       </c>
     </row>
     <row r="17">
@@ -488,19 +488,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>17.064059900166388</v>
+        <v>16.742273180458625</v>
       </c>
       <c r="C17" s="1">
-        <v>21.046925896059058</v>
+        <v>20.794285805291139</v>
       </c>
       <c r="D17" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E17" s="1">
         <v>145</v>
       </c>
       <c r="F17" s="1">
-        <v>30.518041610717773</v>
+        <v>30.151714324951172</v>
       </c>
     </row>
     <row r="18">
@@ -508,19 +508,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>5.3410983136410328</v>
+        <v>16.975265168240394</v>
       </c>
       <c r="C18" s="1">
-        <v>6.587746264414859</v>
+        <v>21.083666997004997</v>
       </c>
       <c r="D18" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E18" s="1">
-        <v>428.5</v>
+        <v>135.11111450195313</v>
       </c>
       <c r="F18" s="1">
-        <v>28.228492736816406</v>
+        <v>28.486377716064453</v>
       </c>
     </row>
     <row r="19">
@@ -528,19 +528,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>16.503447108974868</v>
+        <v>5.3506149702113346</v>
       </c>
       <c r="C19" s="1">
-        <v>20.355461679163472</v>
+        <v>6.6455859827337651</v>
       </c>
       <c r="D19" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E19" s="1">
-        <v>135.11111450195313</v>
+        <v>428.5</v>
       </c>
       <c r="F19" s="1">
-        <v>27.502490997314453</v>
+        <v>28.476335525512695</v>
       </c>
     </row>
     <row r="20">
@@ -548,19 +548,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>25.103399730561776</v>
+        <v>26.817168198696756</v>
       </c>
       <c r="C20" s="1">
-        <v>30.962700259546668</v>
+        <v>33.307535595575338</v>
       </c>
       <c r="D20" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E20" s="1">
         <v>85</v>
       </c>
       <c r="F20" s="1">
-        <v>26.318294525146484</v>
+        <v>28.311405181884766</v>
       </c>
     </row>
     <row r="21">
@@ -568,19 +568,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>10.449726943208056</v>
+        <v>9.8233872607285964</v>
       </c>
       <c r="C21" s="1">
-        <v>12.888762799673986</v>
+        <v>12.200871343666551</v>
       </c>
       <c r="D21" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E21" s="1">
         <v>183.25</v>
       </c>
       <c r="F21" s="1">
-        <v>23.618658065795898</v>
+        <v>22.358097076416016</v>
       </c>
     </row>
     <row r="22">
@@ -588,19 +588,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>14.749227906542888</v>
+        <v>13.281584191060851</v>
       </c>
       <c r="C22" s="1">
-        <v>18.191795983211371</v>
+        <v>16.496030918424331</v>
       </c>
       <c r="D22" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E22" s="1">
         <v>122.46154022216797</v>
       </c>
       <c r="F22" s="1">
-        <v>22.2779541015625</v>
+        <v>20.2012939453125</v>
       </c>
     </row>
     <row r="23">
@@ -608,19 +608,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>13.54171646041997</v>
+        <v>13.179509357821312</v>
       </c>
       <c r="C23" s="1">
-        <v>16.702443285353372</v>
+        <v>16.369251651199761</v>
       </c>
       <c r="D23" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E23" s="1">
         <v>40</v>
       </c>
       <c r="F23" s="1">
-        <v>6.6809773445129395</v>
+        <v>6.5477008819580078</v>
       </c>
     </row>
     <row r="24">
@@ -628,19 +628,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>1.6510577756434233</v>
+        <v>1.5112757105968371</v>
       </c>
       <c r="C24" s="1">
-        <v>2.0364256219340242</v>
+        <v>1.8770389899180633</v>
       </c>
       <c r="D24" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E24" s="1">
         <v>284.66665649414063</v>
       </c>
       <c r="F24" s="1">
-        <v>5.7970247268676758</v>
+        <v>5.3433041572570801</v>
       </c>
     </row>
     <row r="25">
@@ -648,19 +648,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>7.0924650964245028</v>
+        <v>6.6915920387672481</v>
       </c>
       <c r="C25" s="1">
-        <v>8.74789368126436</v>
+        <v>8.3111101554928926</v>
       </c>
       <c r="D25" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E25" s="1">
         <v>56.5</v>
       </c>
       <c r="F25" s="1">
-        <v>4.9425597190856934</v>
+        <v>4.695777416229248</v>
       </c>
     </row>
     <row r="26">
@@ -668,19 +668,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>10.498550219226399</v>
+        <v>9.9464465566313756</v>
       </c>
       <c r="C26" s="1">
-        <v>12.948981782322914</v>
+        <v>12.353713879834064</v>
       </c>
       <c r="D26" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E26" s="1">
         <v>35</v>
       </c>
       <c r="F26" s="1">
-        <v>4.5321435928344727</v>
+        <v>4.3238000869750977</v>
       </c>
     </row>
     <row r="27">
@@ -688,19 +688,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>9.4098409541633092</v>
+        <v>8.7791864503535297</v>
       </c>
       <c r="C27" s="1">
-        <v>11.606160547253296</v>
+        <v>10.903950118828391</v>
       </c>
       <c r="D27" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E27" s="1">
         <v>23</v>
       </c>
       <c r="F27" s="1">
-        <v>2.6694169044494629</v>
+        <v>2.5079085826873779</v>
       </c>
     </row>
     <row r="28">
@@ -708,19 +708,19 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>10.842405759713019</v>
+        <v>11.080093315171419</v>
       </c>
       <c r="C28" s="1">
-        <v>13.373095473989274</v>
+        <v>13.761728929815677</v>
       </c>
       <c r="D28" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E28" s="1">
         <v>5</v>
       </c>
       <c r="F28" s="1">
-        <v>0.66865479946136475</v>
+        <v>0.68808645009994507</v>
       </c>
     </row>
     <row r="29">
@@ -728,13 +728,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="1">
-        <v>18.141526503848553</v>
+        <v>17.59972508986078</v>
       </c>
       <c r="C29" s="1">
-        <v>22.375879706796908</v>
+        <v>21.859260514234933</v>
       </c>
       <c r="D29" s="1">
-        <v>3005</v>
+        <v>3009</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
orshanky revised and outliars removed
</commit_message>
<xml_diff>
--- a/poverty_measurement/output/canasta_diaria.xlsx
+++ b/poverty_measurement/output/canasta_diaria.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>bien</t>
   </si>
@@ -42,12 +42,12 @@
     <t>Carne de res (bistec, carne molida, carne para esmechar)</t>
   </si>
   <si>
+    <t>Lentejas</t>
+  </si>
+  <si>
     <t>Maiz en granos</t>
   </si>
   <si>
-    <t>Lentejas</t>
-  </si>
-  <si>
     <t>Margarina/Mantequilla</t>
   </si>
   <si>
@@ -57,25 +57,22 @@
     <t>Carne de pollo</t>
   </si>
   <si>
+    <t>Platanos</t>
+  </si>
+  <si>
     <t>Frijoles</t>
   </si>
   <si>
-    <t>Platanos</t>
+    <t>Leche en polvo, completa o descremada</t>
   </si>
   <si>
     <t>Huevos (unidades)</t>
   </si>
   <si>
+    <t>Pescado fresco</t>
+  </si>
+  <si>
     <t>Caraotas</t>
-  </si>
-  <si>
-    <t>Leche en polvo, completa o descremada</t>
-  </si>
-  <si>
-    <t>Pescado fresco</t>
-  </si>
-  <si>
-    <t>Hueso de res, pata de res, pata de pollo</t>
   </si>
   <si>
     <t>Papas</t>
@@ -160,7 +157,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F28"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -168,19 +165,19 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>29</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>32</v>
-      </c>
-      <c r="F1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2">
@@ -188,19 +185,19 @@
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>94.976976093559728</v>
+        <v>98.852728790493416</v>
       </c>
       <c r="C2" s="1">
-        <v>117.96357444086199</v>
+        <v>121.37409532839253</v>
       </c>
       <c r="D2" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E2" s="1">
         <v>383</v>
       </c>
       <c r="F2" s="1">
-        <v>451.80047607421875</v>
+        <v>464.86279296875</v>
       </c>
     </row>
     <row r="3">
@@ -208,19 +205,19 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>88.071501905872964</v>
+        <v>93.620393904306553</v>
       </c>
       <c r="C3" s="1">
-        <v>109.386817814227</v>
+        <v>114.94969125460553</v>
       </c>
       <c r="D3" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E3" s="1">
         <v>345</v>
       </c>
       <c r="F3" s="1">
-        <v>377.384521484375</v>
+        <v>396.57644653320313</v>
       </c>
     </row>
     <row r="4">
@@ -228,19 +225,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>19.665394595351557</v>
+        <v>19.696025640934064</v>
       </c>
       <c r="C4" s="1">
-        <v>24.424869165146379</v>
+        <v>24.183321226648587</v>
       </c>
       <c r="D4" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E4" s="1">
         <v>900</v>
       </c>
       <c r="F4" s="1">
-        <v>219.82382202148438</v>
+        <v>217.64988708496094</v>
       </c>
     </row>
     <row r="5">
@@ -248,19 +245,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>29.394199233785663</v>
+        <v>29.431404478367298</v>
       </c>
       <c r="C5" s="1">
-        <v>36.50826673041788</v>
+        <v>36.136687085032463</v>
       </c>
       <c r="D5" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E5" s="1">
         <v>393.5</v>
       </c>
       <c r="F5" s="1">
-        <v>143.6600341796875</v>
+        <v>142.19786071777344</v>
       </c>
     </row>
     <row r="6">
@@ -268,19 +265,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>20.209372464348288</v>
+        <v>21.704589719413431</v>
       </c>
       <c r="C6" s="1">
-        <v>25.100502154881791</v>
+        <v>26.649491610065585</v>
       </c>
       <c r="D6" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E6" s="1">
         <v>368.5</v>
       </c>
       <c r="F6" s="1">
-        <v>92.495353698730469</v>
+        <v>98.203376770019531</v>
       </c>
     </row>
     <row r="7">
@@ -288,19 +285,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="1">
-        <v>45.010208802747741</v>
+        <v>46.558181111530594</v>
       </c>
       <c r="C7" s="1">
-        <v>55.903707537868165</v>
+        <v>57.165414030833908</v>
       </c>
       <c r="D7" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E7" s="1">
         <v>137.5</v>
       </c>
       <c r="F7" s="1">
-        <v>76.867599487304688</v>
+        <v>78.602447509765625</v>
       </c>
     </row>
     <row r="8">
@@ -308,19 +305,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="1">
-        <v>33.815221819460845</v>
+        <v>33.69095706651288</v>
       </c>
       <c r="C8" s="1">
-        <v>41.999278094214674</v>
+        <v>41.366682636481457</v>
       </c>
       <c r="D8" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E8" s="1">
         <v>182.33332824707031</v>
       </c>
       <c r="F8" s="1">
-        <v>76.578681945800781</v>
+        <v>75.425247192382813</v>
       </c>
     </row>
     <row r="9">
@@ -328,19 +325,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="1">
-        <v>28.417130347936801</v>
+        <v>30.1651314147698</v>
       </c>
       <c r="C9" s="1">
-        <v>35.294724975007838</v>
+        <v>37.037577105465758</v>
       </c>
       <c r="D9" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E9" s="1">
         <v>196.5</v>
       </c>
       <c r="F9" s="1">
-        <v>69.354133605957031</v>
+        <v>72.778839111328125</v>
       </c>
     </row>
     <row r="10">
@@ -348,19 +345,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="1">
-        <v>14.018136161076503</v>
+        <v>17.353111109425946</v>
       </c>
       <c r="C10" s="1">
-        <v>17.410845444581959</v>
+        <v>21.306626609576647</v>
       </c>
       <c r="D10" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E10" s="1">
-        <v>355</v>
+        <v>254.5</v>
       </c>
       <c r="F10" s="1">
-        <v>61.808502197265625</v>
+        <v>54.225364685058594</v>
       </c>
     </row>
     <row r="11">
@@ -368,19 +365,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="1">
-        <v>17.566349087224207</v>
+        <v>10.393337275392266</v>
       </c>
       <c r="C11" s="1">
-        <v>21.817806737056085</v>
+        <v>12.761224837953685</v>
       </c>
       <c r="D11" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E11" s="1">
-        <v>254.5</v>
+        <v>355</v>
       </c>
       <c r="F11" s="1">
-        <v>55.526317596435547</v>
+        <v>45.302349090576172</v>
       </c>
     </row>
     <row r="12">
@@ -388,19 +385,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="1">
-        <v>5.620282138927152</v>
+        <v>5.8323734088610575</v>
       </c>
       <c r="C12" s="1">
-        <v>6.9805187861283144</v>
+        <v>7.1611482968093245</v>
       </c>
       <c r="D12" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E12" s="1">
         <v>584</v>
       </c>
       <c r="F12" s="1">
-        <v>40.766231536865234</v>
+        <v>41.82110595703125</v>
       </c>
     </row>
     <row r="13">
@@ -408,19 +405,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="1">
-        <v>28.7704038673875</v>
+        <v>29.662635196921645</v>
       </c>
       <c r="C13" s="1">
-        <v>35.733498839216402</v>
+        <v>36.420598387718201</v>
       </c>
       <c r="D13" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E13" s="1">
         <v>113.375</v>
       </c>
       <c r="F13" s="1">
-        <v>40.512855529785156</v>
+        <v>41.291854858398438</v>
       </c>
     </row>
     <row r="14">
@@ -428,19 +425,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="1">
-        <v>18.268528258614303</v>
+        <v>18.889209435992342</v>
       </c>
       <c r="C14" s="1">
-        <v>22.689929412583172</v>
+        <v>23.192690318951044</v>
       </c>
       <c r="D14" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E14" s="1">
         <v>174</v>
       </c>
       <c r="F14" s="1">
-        <v>39.480476379394531</v>
+        <v>40.355281829833984</v>
       </c>
     </row>
     <row r="15">
@@ -448,19 +445,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>7.4372123992098409</v>
+        <v>17.025249929838282</v>
       </c>
       <c r="C15" s="1">
-        <v>9.2371876337235843</v>
+        <v>20.904069359584522</v>
       </c>
       <c r="D15" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E15" s="1">
-        <v>405.84616088867188</v>
+        <v>164.85714721679688</v>
       </c>
       <c r="F15" s="1">
-        <v>37.48876953125</v>
+        <v>34.46185302734375</v>
       </c>
     </row>
     <row r="16">
@@ -468,19 +465,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>16.781085621918425</v>
+        <v>6.7012290829612366</v>
       </c>
       <c r="C16" s="1">
-        <v>20.842491949860459</v>
+        <v>8.2279531987764507</v>
       </c>
       <c r="D16" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E16" s="1">
-        <v>164.85714721679688</v>
+        <v>405.84616088867188</v>
       </c>
       <c r="F16" s="1">
-        <v>34.360336303710938</v>
+        <v>33.392833709716797</v>
       </c>
     </row>
     <row r="17">
@@ -488,19 +485,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>16.742273180458625</v>
+        <v>6.1035908024798156</v>
       </c>
       <c r="C17" s="1">
-        <v>20.794285805291139</v>
+        <v>7.4941564862446119</v>
       </c>
       <c r="D17" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E17" s="1">
-        <v>145</v>
+        <v>428.5</v>
       </c>
       <c r="F17" s="1">
-        <v>30.151714324951172</v>
+        <v>32.112461090087891</v>
       </c>
     </row>
     <row r="18">
@@ -508,19 +505,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="1">
-        <v>16.975265168240394</v>
+        <v>16.378528225806452</v>
       </c>
       <c r="C18" s="1">
-        <v>21.083666997004997</v>
+        <v>20.110006128588029</v>
       </c>
       <c r="D18" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E18" s="1">
-        <v>135.11111450195313</v>
+        <v>145</v>
       </c>
       <c r="F18" s="1">
-        <v>28.486377716064453</v>
+        <v>29.159509658813477</v>
       </c>
     </row>
     <row r="19">
@@ -528,19 +525,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="1">
-        <v>5.3506149702113346</v>
+        <v>26.759313247537101</v>
       </c>
       <c r="C19" s="1">
-        <v>6.6455859827337651</v>
+        <v>32.855819927748811</v>
       </c>
       <c r="D19" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E19" s="1">
-        <v>428.5</v>
+        <v>85</v>
       </c>
       <c r="F19" s="1">
-        <v>28.476335525512695</v>
+        <v>27.927446365356445</v>
       </c>
     </row>
     <row r="20">
@@ -548,19 +545,19 @@
         <v>19</v>
       </c>
       <c r="B20" s="1">
-        <v>26.817168198696756</v>
+        <v>15.459389871166598</v>
       </c>
       <c r="C20" s="1">
-        <v>33.307535595575338</v>
+        <v>18.981463663039669</v>
       </c>
       <c r="D20" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E20" s="1">
-        <v>85</v>
+        <v>135.11111450195313</v>
       </c>
       <c r="F20" s="1">
-        <v>28.311405181884766</v>
+        <v>25.646066665649414</v>
       </c>
     </row>
     <row r="21">
@@ -568,19 +565,19 @@
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>9.8233872607285964</v>
+        <v>15.005760780906165</v>
       </c>
       <c r="C21" s="1">
-        <v>12.200871343666551</v>
+        <v>18.424485367472453</v>
       </c>
       <c r="D21" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E21" s="1">
-        <v>183.25</v>
+        <v>122.46154022216797</v>
       </c>
       <c r="F21" s="1">
-        <v>22.358097076416016</v>
+        <v>22.562908172607422</v>
       </c>
     </row>
     <row r="22">
@@ -588,19 +585,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>13.281584191060851</v>
+        <v>13.526305961352522</v>
       </c>
       <c r="C22" s="1">
-        <v>16.496030918424331</v>
+        <v>16.607970019822481</v>
       </c>
       <c r="D22" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E22" s="1">
-        <v>122.46154022216797</v>
+        <v>40</v>
       </c>
       <c r="F22" s="1">
-        <v>20.2012939453125</v>
+        <v>6.6431879997253418</v>
       </c>
     </row>
     <row r="23">
@@ -608,19 +605,19 @@
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>13.179509357821312</v>
+        <v>1.8349654508694526</v>
       </c>
       <c r="C23" s="1">
-        <v>16.369251651199761</v>
+        <v>2.2530209428520611</v>
       </c>
       <c r="D23" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E23" s="1">
-        <v>40</v>
+        <v>284.66665649414063</v>
       </c>
       <c r="F23" s="1">
-        <v>6.5477008819580078</v>
+        <v>6.4135994911193848</v>
       </c>
     </row>
     <row r="24">
@@ -628,19 +625,19 @@
         <v>23</v>
       </c>
       <c r="B24" s="1">
-        <v>1.5112757105968371</v>
+        <v>6.8738000714971177</v>
       </c>
       <c r="C24" s="1">
-        <v>1.8770389899180633</v>
+        <v>8.439840540770561</v>
       </c>
       <c r="D24" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E24" s="1">
-        <v>284.66665649414063</v>
+        <v>56.5</v>
       </c>
       <c r="F24" s="1">
-        <v>5.3433041572570801</v>
+        <v>4.7685098648071289</v>
       </c>
     </row>
     <row r="25">
@@ -648,19 +645,19 @@
         <v>24</v>
       </c>
       <c r="B25" s="1">
-        <v>6.6915920387672481</v>
+        <v>10.194652644616943</v>
       </c>
       <c r="C25" s="1">
-        <v>8.3111101554928926</v>
+        <v>12.517274501583268</v>
       </c>
       <c r="D25" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E25" s="1">
-        <v>56.5</v>
+        <v>35</v>
       </c>
       <c r="F25" s="1">
-        <v>4.695777416229248</v>
+        <v>4.3810462951660156</v>
       </c>
     </row>
     <row r="26">
@@ -668,19 +665,19 @@
         <v>25</v>
       </c>
       <c r="B26" s="1">
-        <v>9.9464465566313756</v>
+        <v>9.1769395345641716</v>
       </c>
       <c r="C26" s="1">
-        <v>12.353713879834064</v>
+        <v>11.267698496580124</v>
       </c>
       <c r="D26" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E26" s="1">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="F26" s="1">
-        <v>4.3238000869750977</v>
+        <v>2.5915706157684326</v>
       </c>
     </row>
     <row r="27">
@@ -688,19 +685,19 @@
         <v>26</v>
       </c>
       <c r="B27" s="1">
-        <v>8.7791864503535297</v>
+        <v>10.527313981325396</v>
       </c>
       <c r="C27" s="1">
-        <v>10.903950118828391</v>
+        <v>12.925725298623243</v>
       </c>
       <c r="D27" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E27" s="1">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="F27" s="1">
-        <v>2.5079085826873779</v>
+        <v>0.6462862491607666</v>
       </c>
     </row>
     <row r="28">
@@ -708,38 +705,18 @@
         <v>27</v>
       </c>
       <c r="B28" s="1">
-        <v>11.080093315171419</v>
+        <v>17.385177094929961</v>
       </c>
       <c r="C28" s="1">
-        <v>13.761728929815677</v>
+        <v>21.345998065045443</v>
       </c>
       <c r="D28" s="1">
-        <v>3009</v>
+        <v>2976</v>
       </c>
       <c r="E28" s="1">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F28" s="1">
-        <v>0.68808645009994507</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1">
-        <v>17.59972508986078</v>
-      </c>
-      <c r="C29" s="1">
-        <v>21.859260514234933</v>
-      </c>
-      <c r="D29" s="1">
-        <v>3009</v>
-      </c>
-      <c r="E29" s="1">
-        <v>0</v>
-      </c>
-      <c r="F29" s="1">
         <v>0</v>
       </c>
     </row>

</xml_diff>